<commit_message>
Update DR# 712 AllHome (Javelin DNA Printer with MS)_01_24_2022.xlsx
</commit_message>
<xml_diff>
--- a/DR# 712 AllHome (Javelin DNA Printer with MS)_01_24_2022.xlsx
+++ b/DR# 712 AllHome (Javelin DNA Printer with MS)_01_24_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Ponio IV\Documents\GitHub\Delivery-Receipt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Dropbox\PC\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B54FF19-9270-4A86-AB9C-03B18D5F7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D6454C-98AB-4A7D-9C06-BA7B54E0E4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Address: South Super Highway, Alabang, Muntinlupa, Metro Manila</t>
   </si>
   <si>
-    <t>TO:  AllHome</t>
-  </si>
-  <si>
     <t>Printer</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
       </rPr>
       <t xml:space="preserve"> 000712</t>
     </r>
+  </si>
+  <si>
+    <t>TO:  AllDay</t>
   </si>
 </sst>
 </file>
@@ -943,13 +943,13 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
@@ -1020,8 +1020,8 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:9" ht="31.5">
+    <row r="13" spans="1:9" ht="15" thickBot="1"/>
+    <row r="14" spans="1:9" ht="31.2">
       <c r="A14" s="6" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="30">
+    <row r="15" spans="1:9" ht="28.8">
       <c r="A15" s="12" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+    <row r="27" spans="1:5" ht="15" thickBot="1">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1165,13 +1165,13 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
@@ -1242,8 +1242,8 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:9" ht="31.5">
+    <row r="13" spans="1:9" ht="15" thickBot="1"/>
+    <row r="14" spans="1:9" ht="31.2">
       <c r="A14" s="6" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+    <row r="27" spans="1:5" ht="15" thickBot="1">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1383,16 +1383,16 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -1432,18 +1432,18 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="18.75">
+    <row r="9" spans="1:13" ht="18">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1470,7 +1470,7 @@
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75">
+    <row r="12" spans="1:13" ht="18">
       <c r="A12" s="23"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -1478,14 +1478,14 @@
       <c r="E12" s="23"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="19.5" thickBot="1">
+    <row r="13" spans="1:13" ht="18.600000000000001" thickBot="1">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="37.5">
+    <row r="14" spans="1:13" ht="36">
       <c r="A14" s="43" t="s">
         <v>1</v>
       </c>
@@ -1502,12 +1502,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="37.5">
+    <row r="15" spans="1:13" ht="36">
       <c r="A15" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>27</v>
       </c>
       <c r="C15" s="37">
         <v>1</v>
@@ -1519,12 +1519,12 @@
         <v>44585</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75">
+    <row r="16" spans="1:13" ht="18">
       <c r="A16" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="37">
         <v>2</v>
@@ -1536,12 +1536,12 @@
         <v>44585</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75">
+    <row r="17" spans="1:5" ht="18">
       <c r="A17" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="29">
         <v>2</v>
@@ -1553,28 +1553,28 @@
         <v>44585</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18.75">
+    <row r="18" spans="1:5" ht="18">
       <c r="A18" s="28"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="31"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75">
+    <row r="19" spans="1:5" ht="18">
       <c r="A19" s="28"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="E19" s="31"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75">
+    <row r="20" spans="1:5" ht="18">
       <c r="A20" s="28"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75">
+    <row r="21" spans="1:5" ht="18">
       <c r="A21" s="33" t="s">
         <v>22</v>
       </c>
@@ -1583,7 +1583,7 @@
       <c r="D21" s="30"/>
       <c r="E21" s="31"/>
     </row>
-    <row r="22" spans="1:5" ht="19.5" thickBot="1">
+    <row r="22" spans="1:5" ht="18.600000000000001" thickBot="1">
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>

</xml_diff>